<commit_message>
updated paths in the config
</commit_message>
<xml_diff>
--- a/Asset Twin Setup/config/Config_Sheet.xlsx
+++ b/Asset Twin Setup/config/Config_Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://invicara-my.sharepoint.com/personal/vivek_mandal_ext_invicara_com/Documents/Documents/oneClickData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\code\Twinit-IPA-Core-Digital-Buildings\Asset Twin Setup\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{779A2EDC-5BA2-4025-B03B-C5C41BEBD4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A38407D5-F91C-48D3-BE7B-B2B4EF28C021}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A717004C-BB26-4313-863C-E5431D760304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="1480" windowWidth="14400" windowHeight="7270" tabRatio="704" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="270" windowWidth="24765" windowHeight="15240" tabRatio="704" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -2774,16 +2774,16 @@
     <t>contained_by_spatial_structure</t>
   </si>
   <si>
-    <t>C:/projects/ClientApplicationConfig/</t>
-  </si>
-  <si>
     <t>Script Path</t>
   </si>
   <si>
     <t>BIMPK Path</t>
   </si>
   <si>
-    <t>C:/Users/bimpk.bimpk</t>
+    <t>C:/projects/Twinit-IPA-Core-Digital-Buildings/Asset Twin Setup/scripts</t>
+  </si>
+  <si>
+    <t>C:/projects/Twinit-IPA-Core-Digital-Buildings/model</t>
   </si>
 </sst>
 </file>
@@ -3315,19 +3315,19 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.7265625" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" customWidth="1"/>
-    <col min="6" max="6" width="13.7265625" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" customWidth="1"/>
-    <col min="8" max="8" width="13.7265625" customWidth="1"/>
-    <col min="9" max="9" width="16.453125" customWidth="1"/>
-    <col min="10" max="10" width="16.26953125" customWidth="1"/>
-    <col min="1024" max="1024" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="1024" max="1024" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -3485,16 +3485,16 @@
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="6" max="6" width="24.54296875" customWidth="1"/>
-    <col min="7" max="7" width="23.54296875" customWidth="1"/>
-    <col min="8" max="8" width="22.54296875" customWidth="1"/>
-    <col min="9" max="9" width="23.453125" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -3518,7 +3518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -3560,19 +3560,19 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="32.7265625" customWidth="1"/>
-    <col min="3" max="3" width="27.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" customWidth="1"/>
-    <col min="5" max="5" width="30.1796875" customWidth="1"/>
-    <col min="6" max="6" width="36.1796875" customWidth="1"/>
-    <col min="7" max="7" width="30.54296875" customWidth="1"/>
-    <col min="8" max="8" width="27.1796875" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" customWidth="1"/>
+    <col min="6" max="6" width="36.140625" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" customWidth="1"/>
+    <col min="8" max="8" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>896</v>
       </c>
@@ -3624,7 +3624,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>58</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>59</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>24</v>
       </c>
@@ -3707,7 +3707,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>25</v>
       </c>
@@ -3722,7 +3722,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>60</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>61</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>62</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>28</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
       <c r="F12" s="2" t="s">
         <v>93</v>
@@ -3784,7 +3784,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="D13" s="2"/>
       <c r="F13" s="2" t="s">
         <v>95</v>
@@ -3793,7 +3793,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
       <c r="F14" s="2" t="s">
         <v>97</v>
@@ -3821,19 +3821,19 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.54296875" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.26953125" customWidth="1"/>
-    <col min="14" max="14" width="12.26953125" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -3899,7 +3899,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>679</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>680</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>681</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>906</v>
       </c>
@@ -3994,20 +3994,20 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="46" customWidth="1"/>
-    <col min="3" max="3" width="23.81640625" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="16.26953125" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="str">
         <f>C2</f>
         <v>EXAM 1-4</v>
@@ -4060,7 +4060,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A66" si="0">C3</f>
         <v>EXAM 1-3</v>
@@ -4084,7 +4084,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>EXAM 1-2</v>
@@ -4108,7 +4108,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>EXAM 1-1</v>
@@ -4132,7 +4132,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>CONSULT 1</v>
@@ -4156,7 +4156,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>CONSULT 2</v>
@@ -4180,7 +4180,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>EXAM 2-1</v>
@@ -4204,7 +4204,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>EXAM 2-2</v>
@@ -4228,7 +4228,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>EXAM 2-3</v>
@@ -4252,7 +4252,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>EXAM 2-4</v>
@@ -4276,7 +4276,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>EXAM 3-4</v>
@@ -4300,7 +4300,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>EXAM 3-3</v>
@@ -4327,7 +4327,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>EXAM 3-2</v>
@@ -4354,7 +4354,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>EXAM 3-1</v>
@@ -4381,7 +4381,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>CONSULT 3</v>
@@ -4408,7 +4408,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>PATIENT RESTROOM</v>
@@ -4435,7 +4435,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>PUBLIC RESTROOM</v>
@@ -4462,7 +4462,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>JANITOR - 2</v>
@@ -4489,7 +4489,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>RECEPTION</v>
@@ -4516,7 +4516,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>LAB</v>
@@ -4543,7 +4543,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>TRIAGE</v>
@@ -4570,7 +4570,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>TREATMENT ROOM</v>
@@ -4597,7 +4597,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>MEDICAL GASES</v>
@@ -4624,7 +4624,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>XRAY</v>
@@ -4651,7 +4651,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>XRAY DEVELOPING</v>
@@ -4678,7 +4678,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>PHARMACY</v>
@@ -4705,7 +4705,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>ENTRY - 2</v>
@@ -4732,7 +4732,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>STAFF RESTROOM</v>
@@ -4759,7 +4759,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>SHOWER/LOCKER</v>
@@ -4786,7 +4786,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>SUPPLIES</v>
@@ -4813,7 +4813,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>ELECTRICAL</v>
@@ -4840,7 +4840,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>STAIRS</v>
@@ -4867,7 +4867,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>MRL ELEVATOR</v>
@@ -4894,7 +4894,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>LOBBY</v>
@@ -4921,7 +4921,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>PATIENT COORIDOR</v>
@@ -4948,7 +4948,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>NURSE STATION - 2</v>
@@ -4975,7 +4975,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>STAFF ENTRY</v>
@@ -5002,7 +5002,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>OUTPATIENT CENTER</v>
@@ -5029,7 +5029,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>ENTRY</v>
@@ -5056,7 +5056,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>MECH</v>
@@ -5080,7 +5080,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
         <f t="shared" si="0"/>
         <v>DR OFFICE - 1</v>
@@ -5107,7 +5107,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
         <f t="shared" si="0"/>
         <v>DR OFFICE - 2</v>
@@ -5134,7 +5134,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
         <f t="shared" si="0"/>
         <v>DR OFFICE - 3</v>
@@ -5161,7 +5161,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
         <f t="shared" si="0"/>
         <v>DR OFFICE - 4</v>
@@ -5188,7 +5188,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="str">
         <f t="shared" si="0"/>
         <v>DR OFFICE - 5</v>
@@ -5215,7 +5215,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="str">
         <f t="shared" si="0"/>
         <v>RESTROOM - 1</v>
@@ -5242,7 +5242,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="str">
         <f t="shared" si="0"/>
         <v>RESTROOM -2</v>
@@ -5269,7 +5269,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
         <f t="shared" si="0"/>
         <v>VISITING DR</v>
@@ -5296,7 +5296,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="str">
         <f t="shared" si="0"/>
         <v>NURSING OFFICE</v>
@@ -5320,7 +5320,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="str">
         <f t="shared" si="0"/>
         <v>ACCOUNTING</v>
@@ -5347,7 +5347,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="str">
         <f t="shared" si="0"/>
         <v>AV</v>
@@ -5371,7 +5371,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="str">
         <f t="shared" si="0"/>
         <v>BREAK ROOM</v>
@@ -5398,7 +5398,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
         <f t="shared" si="0"/>
         <v>STAIR</v>
@@ -5425,7 +5425,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
         <f t="shared" si="0"/>
         <v>ELECTRIC COMMUNICATIONS</v>
@@ -5452,7 +5452,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="str">
         <f t="shared" si="0"/>
         <v>COORIDOR</v>
@@ -5476,7 +5476,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
         <f t="shared" si="0"/>
         <v>RECORDS</v>
@@ -5503,7 +5503,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
         <f t="shared" si="0"/>
         <v>SOILED LINEN</v>
@@ -5530,7 +5530,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
         <f t="shared" si="0"/>
         <v>CLEAN LINEN</v>
@@ -5557,7 +5557,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="str">
         <f t="shared" si="0"/>
         <v>CONFERENCE</v>
@@ -5584,7 +5584,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="str">
         <f t="shared" si="0"/>
         <v>UPPER LOBBY</v>
@@ -5611,7 +5611,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="str">
         <f t="shared" si="0"/>
         <v>NURSE STATION</v>
@@ -5638,7 +5638,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="str">
         <f t="shared" si="0"/>
         <v>ELEV CONTROLS</v>
@@ -5665,7 +5665,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="str">
         <f t="shared" si="0"/>
         <v>DR SCRUB</v>
@@ -5692,7 +5692,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="str">
         <f t="shared" si="0"/>
         <v>JANITOR - 1</v>
@@ -5719,7 +5719,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="str">
         <f t="shared" si="0"/>
         <v>JANITOR - 3</v>
@@ -5746,7 +5746,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="str">
         <f t="shared" ref="A67:A72" si="1">C67</f>
         <v>STAFF ENTRANCE</v>
@@ -5770,7 +5770,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="str">
         <f t="shared" si="1"/>
         <v>CLOSET</v>
@@ -5794,7 +5794,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="str">
         <f t="shared" si="1"/>
         <v>Room-1</v>
@@ -5818,7 +5818,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="str">
         <f t="shared" si="1"/>
         <v>Room-2</v>
@@ -5842,7 +5842,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="str">
         <f t="shared" si="1"/>
         <v>Room-3</v>
@@ -5866,7 +5866,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="str">
         <f t="shared" si="1"/>
         <v>Room-4</v>
@@ -5912,19 +5912,19 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" customWidth="1"/>
-    <col min="5" max="5" width="22.453125" customWidth="1"/>
-    <col min="6" max="6" width="47.26953125" customWidth="1"/>
-    <col min="8" max="8" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="47.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -5950,7 +5950,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>106</v>
       </c>
@@ -5973,7 +5973,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -5993,7 +5993,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>107</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>108</v>
       </c>
@@ -6032,7 +6032,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -6040,7 +6040,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -6048,7 +6048,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>109</v>
       </c>
@@ -6056,7 +6056,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -6064,7 +6064,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -6080,7 +6080,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -6088,7 +6088,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>907</v>
       </c>
@@ -6123,23 +6123,23 @@
       <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="5" width="7.453125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.54296875" customWidth="1"/>
+    <col min="4" max="5" width="7.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.5703125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="49" customWidth="1"/>
-    <col min="10" max="10" width="13.26953125" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
-    <col min="12" max="12" width="14.453125" customWidth="1"/>
-    <col min="14" max="14" width="17.54296875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>106</v>
       </c>
@@ -6183,7 +6183,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -6226,7 +6226,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>117</v>
       </c>
@@ -6266,7 +6266,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -6346,7 +6346,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -6386,7 +6386,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>134</v>
       </c>
@@ -6426,7 +6426,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>136</v>
       </c>
@@ -6466,7 +6466,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>138</v>
       </c>
@@ -6506,7 +6506,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>140</v>
       </c>
@@ -6546,7 +6546,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -6586,7 +6586,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>144</v>
       </c>
@@ -6626,7 +6626,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>146</v>
       </c>
@@ -6666,7 +6666,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>148</v>
       </c>
@@ -6706,7 +6706,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>150</v>
       </c>
@@ -6746,7 +6746,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>152</v>
       </c>
@@ -6786,7 +6786,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>154</v>
       </c>
@@ -6826,7 +6826,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>156</v>
       </c>
@@ -6866,7 +6866,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>158</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>160</v>
       </c>
@@ -6946,7 +6946,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>162</v>
       </c>
@@ -6986,7 +6986,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>164</v>
       </c>
@@ -7026,7 +7026,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>166</v>
       </c>
@@ -7066,7 +7066,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>168</v>
       </c>
@@ -7106,7 +7106,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>172</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>174</v>
       </c>
@@ -7186,7 +7186,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>176</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>178</v>
       </c>
@@ -7266,7 +7266,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>180</v>
       </c>
@@ -7306,7 +7306,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>182</v>
       </c>
@@ -7346,7 +7346,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>184</v>
       </c>
@@ -7386,7 +7386,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>186</v>
       </c>
@@ -7426,7 +7426,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>188</v>
       </c>
@@ -7466,7 +7466,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>190</v>
       </c>
@@ -7506,7 +7506,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>192</v>
       </c>
@@ -7549,7 +7549,7 @@
         <v>2741</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>194</v>
       </c>
@@ -7592,7 +7592,7 @@
         <v>2811</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>196</v>
       </c>
@@ -7635,7 +7635,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>198</v>
       </c>
@@ -7678,7 +7678,7 @@
         <v>2701</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>202</v>
       </c>
@@ -7721,7 +7721,7 @@
         <v>2821</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>204</v>
       </c>
@@ -7764,7 +7764,7 @@
         <v>2816</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>206</v>
       </c>
@@ -7807,7 +7807,7 @@
         <v>2796</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>208</v>
       </c>
@@ -7850,7 +7850,7 @@
         <v>2796</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>210</v>
       </c>
@@ -7893,7 +7893,7 @@
         <v>2621</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>212</v>
       </c>
@@ -7936,7 +7936,7 @@
         <v>2676</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>214</v>
       </c>
@@ -7976,7 +7976,7 @@
         <v>2671</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>217</v>
       </c>
@@ -8016,7 +8016,7 @@
         <v>2731</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>219</v>
       </c>
@@ -8059,7 +8059,7 @@
         <v>2641</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>221</v>
       </c>
@@ -8102,7 +8102,7 @@
         <v>2646</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>223</v>
       </c>
@@ -8145,7 +8145,7 @@
         <v>2856</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>225</v>
       </c>
@@ -8188,7 +8188,7 @@
         <v>2656</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>228</v>
       </c>
@@ -8231,7 +8231,7 @@
         <v>2666</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>230</v>
       </c>
@@ -8274,7 +8274,7 @@
         <v>2636</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>232</v>
       </c>
@@ -8317,7 +8317,7 @@
         <v>2726</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>236</v>
       </c>
@@ -8360,7 +8360,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>238</v>
       </c>
@@ -8403,7 +8403,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>242</v>
       </c>
@@ -8446,7 +8446,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>246</v>
       </c>
@@ -8489,7 +8489,7 @@
         <v>2831</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>248</v>
       </c>
@@ -8532,7 +8532,7 @@
         <v>2826</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>250</v>
       </c>
@@ -8575,7 +8575,7 @@
         <v>2861</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>252</v>
       </c>
@@ -8618,7 +8618,7 @@
         <v>2686</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>254</v>
       </c>
@@ -8661,7 +8661,7 @@
         <v>2701</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>256</v>
       </c>
@@ -8704,7 +8704,7 @@
         <v>2776</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>258</v>
       </c>
@@ -8747,7 +8747,7 @@
         <v>2771</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>260</v>
       </c>
@@ -8790,7 +8790,7 @@
         <v>2816</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>262</v>
       </c>
@@ -8833,7 +8833,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>264</v>
       </c>
@@ -8876,7 +8876,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>266</v>
       </c>
@@ -8919,7 +8919,7 @@
         <v>2706</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>269</v>
       </c>
@@ -8962,7 +8962,7 @@
         <v>2836</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>272</v>
       </c>
@@ -9005,7 +9005,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>275</v>
       </c>
@@ -9048,7 +9048,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>278</v>
       </c>
@@ -9091,7 +9091,7 @@
         <v>2821</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>280</v>
       </c>
@@ -9134,7 +9134,7 @@
         <v>2841</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>282</v>
       </c>
@@ -9174,7 +9174,7 @@
         <v>2468</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>286</v>
       </c>
@@ -9214,7 +9214,7 @@
         <v>2736</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>288</v>
       </c>
@@ -9257,7 +9257,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>290</v>
       </c>
@@ -9297,7 +9297,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>295</v>
       </c>
@@ -9337,7 +9337,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>297</v>
       </c>
@@ -9377,7 +9377,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>299</v>
       </c>
@@ -9417,7 +9417,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>301</v>
       </c>
@@ -9457,7 +9457,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>303</v>
       </c>
@@ -9497,7 +9497,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>305</v>
       </c>
@@ -9540,7 +9540,7 @@
         <v>2586</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>307</v>
       </c>
@@ -9583,7 +9583,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>309</v>
       </c>
@@ -9626,7 +9626,7 @@
         <v>2606</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>311</v>
       </c>
@@ -9669,7 +9669,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>313</v>
       </c>
@@ -9712,7 +9712,7 @@
         <v>2576</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>315</v>
       </c>
@@ -9755,7 +9755,7 @@
         <v>2571</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>317</v>
       </c>
@@ -9798,7 +9798,7 @@
         <v>2666</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>321</v>
       </c>
@@ -9841,7 +9841,7 @@
         <v>2636</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>323</v>
       </c>
@@ -9884,7 +9884,7 @@
         <v>2636</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>326</v>
       </c>
@@ -9927,7 +9927,7 @@
         <v>2636</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>328</v>
       </c>
@@ -9970,7 +9970,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>331</v>
       </c>
@@ -10013,7 +10013,7 @@
         <v>2871</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>333</v>
       </c>
@@ -10056,7 +10056,7 @@
         <v>2631</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>335</v>
       </c>
@@ -10099,7 +10099,7 @@
         <v>2566</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>337</v>
       </c>
@@ -10142,7 +10142,7 @@
         <v>2611</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>339</v>
       </c>
@@ -10185,7 +10185,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>341</v>
       </c>
@@ -10228,7 +10228,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>345</v>
       </c>
@@ -10271,7 +10271,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>349</v>
       </c>
@@ -10314,7 +10314,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>352</v>
       </c>
@@ -10357,7 +10357,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>354</v>
       </c>
@@ -10400,7 +10400,7 @@
         <v>2557</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>356</v>
       </c>
@@ -10443,7 +10443,7 @@
         <v>2631</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>359</v>
       </c>
@@ -10486,7 +10486,7 @@
         <v>2945</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>362</v>
       </c>
@@ -10529,7 +10529,7 @@
         <v>2945</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>364</v>
       </c>
@@ -10572,7 +10572,7 @@
         <v>2945</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>366</v>
       </c>
@@ -10615,7 +10615,7 @@
         <v>2955</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>368</v>
       </c>
@@ -10658,7 +10658,7 @@
         <v>2955</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>370</v>
       </c>
@@ -10701,7 +10701,7 @@
         <v>2955</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>372</v>
       </c>
@@ -10744,7 +10744,7 @@
         <v>2937</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>374</v>
       </c>
@@ -10787,7 +10787,7 @@
         <v>2937</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>376</v>
       </c>
@@ -10830,7 +10830,7 @@
         <v>2921</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>378</v>
       </c>
@@ -10873,7 +10873,7 @@
         <v>2945</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>381</v>
       </c>
@@ -10916,7 +10916,7 @@
         <v>2960</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>383</v>
       </c>
@@ -10959,7 +10959,7 @@
         <v>2937</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>385</v>
       </c>
@@ -11002,7 +11002,7 @@
         <v>2882</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>387</v>
       </c>
@@ -11045,7 +11045,7 @@
         <v>2945</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>389</v>
       </c>
@@ -11088,7 +11088,7 @@
         <v>2960</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>391</v>
       </c>
@@ -11131,7 +11131,7 @@
         <v>2921</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>393</v>
       </c>
@@ -11174,7 +11174,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>396</v>
       </c>
@@ -11217,7 +11217,7 @@
         <v>2945</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>401</v>
       </c>
@@ -11260,7 +11260,7 @@
         <v>2950</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>403</v>
       </c>
@@ -11303,7 +11303,7 @@
         <v>2937</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>405</v>
       </c>
@@ -11346,7 +11346,7 @@
         <v>2929</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>407</v>
       </c>
@@ -11386,7 +11386,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>412</v>
       </c>
@@ -11426,7 +11426,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>414</v>
       </c>
@@ -11466,7 +11466,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>416</v>
       </c>
@@ -11506,7 +11506,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>418</v>
       </c>
@@ -11546,7 +11546,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>420</v>
       </c>
@@ -11586,7 +11586,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>422</v>
       </c>
@@ -11626,7 +11626,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>424</v>
       </c>
@@ -11666,7 +11666,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>426</v>
       </c>
@@ -11706,7 +11706,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>428</v>
       </c>
@@ -11746,7 +11746,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>430</v>
       </c>
@@ -11786,7 +11786,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>434</v>
       </c>
@@ -11826,7 +11826,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>436</v>
       </c>
@@ -11866,7 +11866,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>438</v>
       </c>
@@ -11906,7 +11906,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>440</v>
       </c>
@@ -11946,7 +11946,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>442</v>
       </c>
@@ -11986,7 +11986,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>444</v>
       </c>
@@ -12026,7 +12026,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>446</v>
       </c>
@@ -12066,7 +12066,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>448</v>
       </c>
@@ -12109,7 +12109,7 @@
         <v>2646</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>452</v>
       </c>
@@ -12152,7 +12152,7 @@
         <v>2706</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>459</v>
       </c>
@@ -12195,7 +12195,7 @@
         <v>2706</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>461</v>
       </c>
@@ -12238,7 +12238,7 @@
         <v>2706</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>463</v>
       </c>
@@ -12281,7 +12281,7 @@
         <v>2706</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>465</v>
       </c>
@@ -12324,7 +12324,7 @@
         <v>2706</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>467</v>
       </c>
@@ -12367,7 +12367,7 @@
         <v>2706</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>469</v>
       </c>
@@ -12410,7 +12410,7 @@
         <v>2706</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>471</v>
       </c>
@@ -12453,7 +12453,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>473</v>
       </c>
@@ -12496,7 +12496,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>475</v>
       </c>
@@ -12539,7 +12539,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>477</v>
       </c>
@@ -12582,7 +12582,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>479</v>
       </c>
@@ -12625,7 +12625,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>481</v>
       </c>
@@ -12668,7 +12668,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>483</v>
       </c>
@@ -12711,7 +12711,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>485</v>
       </c>
@@ -12754,7 +12754,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>489</v>
       </c>
@@ -12797,7 +12797,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>491</v>
       </c>
@@ -12840,7 +12840,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>493</v>
       </c>
@@ -12883,7 +12883,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>495</v>
       </c>
@@ -12926,7 +12926,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>497</v>
       </c>
@@ -12969,7 +12969,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>499</v>
       </c>
@@ -13012,7 +13012,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>501</v>
       </c>
@@ -13055,7 +13055,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>503</v>
       </c>
@@ -13098,7 +13098,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>505</v>
       </c>
@@ -13141,7 +13141,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>507</v>
       </c>
@@ -13184,7 +13184,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>509</v>
       </c>
@@ -13227,7 +13227,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>511</v>
       </c>
@@ -13270,7 +13270,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>513</v>
       </c>
@@ -13313,7 +13313,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>515</v>
       </c>
@@ -13356,7 +13356,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>517</v>
       </c>
@@ -13399,7 +13399,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>519</v>
       </c>
@@ -13442,7 +13442,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>521</v>
       </c>
@@ -13485,7 +13485,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>523</v>
       </c>
@@ -13528,7 +13528,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>525</v>
       </c>
@@ -13571,7 +13571,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>527</v>
       </c>
@@ -13614,7 +13614,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>529</v>
       </c>
@@ -13657,7 +13657,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>531</v>
       </c>
@@ -13700,7 +13700,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>533</v>
       </c>
@@ -13743,7 +13743,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>535</v>
       </c>
@@ -13783,7 +13783,7 @@
         <v>2945</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>542</v>
       </c>
@@ -13823,7 +13823,7 @@
         <v>2950</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>544</v>
       </c>
@@ -13863,7 +13863,7 @@
         <v>2937</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>546</v>
       </c>
@@ -13903,7 +13903,7 @@
         <v>2929</v>
       </c>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>548</v>
       </c>
@@ -13940,7 +13940,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>554</v>
       </c>
@@ -13977,7 +13977,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>556</v>
       </c>
@@ -14014,7 +14014,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>558</v>
       </c>
@@ -14051,7 +14051,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>560</v>
       </c>
@@ -14091,7 +14091,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>564</v>
       </c>
@@ -14131,7 +14131,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>569</v>
       </c>
@@ -14171,7 +14171,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>571</v>
       </c>
@@ -14211,7 +14211,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>573</v>
       </c>
@@ -14251,7 +14251,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>575</v>
       </c>
@@ -14291,7 +14291,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>577</v>
       </c>
@@ -14331,7 +14331,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>579</v>
       </c>
@@ -14371,7 +14371,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>581</v>
       </c>
@@ -14411,7 +14411,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>583</v>
       </c>
@@ -14451,7 +14451,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>585</v>
       </c>
@@ -14491,7 +14491,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>587</v>
       </c>
@@ -14531,7 +14531,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>589</v>
       </c>
@@ -14571,7 +14571,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>591</v>
       </c>
@@ -14611,7 +14611,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>595</v>
       </c>
@@ -14651,7 +14651,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>599</v>
       </c>
@@ -14691,7 +14691,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>601</v>
       </c>
@@ -14731,7 +14731,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>603</v>
       </c>
@@ -14771,7 +14771,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>605</v>
       </c>
@@ -14811,7 +14811,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>607</v>
       </c>
@@ -14851,7 +14851,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>609</v>
       </c>
@@ -14891,7 +14891,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>611</v>
       </c>
@@ -14931,7 +14931,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>614</v>
       </c>
@@ -14971,7 +14971,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>616</v>
       </c>
@@ -15011,7 +15011,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>618</v>
       </c>
@@ -15051,7 +15051,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>622</v>
       </c>
@@ -15088,7 +15088,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>625</v>
       </c>
@@ -15125,7 +15125,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>627</v>
       </c>
@@ -15162,7 +15162,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>629</v>
       </c>
@@ -15202,7 +15202,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>631</v>
       </c>
@@ -15242,7 +15242,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>633</v>
       </c>
@@ -15282,7 +15282,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>635</v>
       </c>
@@ -15322,7 +15322,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>637</v>
       </c>
@@ -15359,7 +15359,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>639</v>
       </c>
@@ -15396,7 +15396,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>641</v>
       </c>
@@ -15436,7 +15436,7 @@
         <v>2945</v>
       </c>
     </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>648</v>
       </c>
@@ -15476,7 +15476,7 @@
         <v>2945</v>
       </c>
     </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>650</v>
       </c>
@@ -15516,7 +15516,7 @@
         <v>2950</v>
       </c>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>652</v>
       </c>
@@ -15556,7 +15556,7 @@
         <v>2950</v>
       </c>
     </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>654</v>
       </c>
@@ -15596,7 +15596,7 @@
         <v>2937</v>
       </c>
     </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>656</v>
       </c>
@@ -15636,7 +15636,7 @@
         <v>2937</v>
       </c>
     </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>658</v>
       </c>
@@ -15676,7 +15676,7 @@
         <v>2929</v>
       </c>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>660</v>
       </c>
@@ -15716,7 +15716,7 @@
         <v>2929</v>
       </c>
     </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>662</v>
       </c>
@@ -15756,7 +15756,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>667</v>
       </c>
@@ -15796,7 +15796,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>669</v>
       </c>
@@ -15836,7 +15836,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>671</v>
       </c>
@@ -15876,7 +15876,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>673</v>
       </c>
@@ -15916,7 +15916,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>675</v>
       </c>
@@ -15970,16 +15970,16 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.453125" customWidth="1"/>
-    <col min="2" max="2" width="64.1796875" customWidth="1"/>
-    <col min="3" max="3" width="66.7265625" customWidth="1"/>
-    <col min="4" max="4" width="26.81640625" customWidth="1"/>
-    <col min="5" max="5" width="34.26953125" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" customWidth="1"/>
+    <col min="2" max="2" width="64.140625" customWidth="1"/>
+    <col min="3" max="3" width="66.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -15996,7 +15996,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>294</v>
       </c>
@@ -16013,7 +16013,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -16030,7 +16030,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>294</v>
       </c>
@@ -16047,7 +16047,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>294</v>
       </c>
@@ -16064,7 +16064,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>294</v>
       </c>
@@ -16081,7 +16081,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>294</v>
       </c>
@@ -16098,7 +16098,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>294</v>
       </c>
@@ -16115,7 +16115,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>294</v>
       </c>
@@ -16132,7 +16132,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -16149,7 +16149,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -16166,7 +16166,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -16183,7 +16183,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -16200,7 +16200,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -16217,7 +16217,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -16234,7 +16234,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -16251,7 +16251,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -16268,7 +16268,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -16285,7 +16285,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -16302,7 +16302,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -16319,7 +16319,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -16336,7 +16336,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -16353,7 +16353,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -16370,7 +16370,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -16387,7 +16387,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>541</v>
       </c>
@@ -16404,7 +16404,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -16421,7 +16421,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -16438,7 +16438,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>400</v>
       </c>
@@ -16455,7 +16455,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>458</v>
       </c>
@@ -16472,7 +16472,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>458</v>
       </c>
@@ -16489,7 +16489,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>553</v>
       </c>
@@ -16506,7 +16506,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>553</v>
       </c>
@@ -16523,7 +16523,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>553</v>
       </c>
@@ -16540,7 +16540,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>553</v>
       </c>
@@ -16557,7 +16557,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>553</v>
       </c>
@@ -16574,7 +16574,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>553</v>
       </c>
@@ -16591,7 +16591,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>553</v>
       </c>
@@ -16608,7 +16608,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>553</v>
       </c>
@@ -16625,7 +16625,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>647</v>
       </c>
@@ -16642,7 +16642,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>115</v>
       </c>
@@ -16659,7 +16659,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>115</v>
       </c>
@@ -16676,7 +16676,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>115</v>
       </c>
@@ -16693,7 +16693,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>115</v>
       </c>
@@ -16710,7 +16710,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>39</v>
       </c>
@@ -16727,7 +16727,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -16744,7 +16744,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -16776,26 +16776,26 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.54296875" customWidth="1"/>
-    <col min="2" max="2" width="59.36328125" customWidth="1"/>
+    <col min="1" max="1" width="60.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>908</v>
+      </c>
+      <c r="B1" t="s">
         <v>909</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>910</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>908</v>
       </c>
       <c r="B2" t="s">
         <v>911</v>
@@ -16807,6 +16807,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -16817,15 +16826,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17095,6 +17095,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46591259-1875-401E-86A5-38FE831D6A47}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{666BD942-0103-4387-A6D7-5914FC29A59A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -17102,14 +17110,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="11ebf1cd-3aa0-4579-80fd-628e9a673e65"/>
     <ds:schemaRef ds:uri="95f9ca3d-78ae-45a7-840a-8d062c71c3e5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46591259-1875-401E-86A5-38FE831D6A47}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>